<commit_message>
2017-02-13 snapshot - chunk 22
</commit_message>
<xml_diff>
--- a/www.eia.gov/petroleum/drilling/xls/duc-data.xlsx
+++ b/www.eia.gov/petroleum/drilling/xls/duc-data.xlsx
@@ -15,15 +15,12 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="webSummary" sheetId="5" state="hidden" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Data!$A$1:$AF$41</definedName>
-  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
   <si>
     <t>Haynesville</t>
   </si>
@@ -62,6 +59,21 @@
   </si>
   <si>
     <t xml:space="preserve">  Eagle Ford</t>
+  </si>
+  <si>
+    <t>Bakken</t>
+  </si>
+  <si>
+    <t>Eagle Ford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcellus </t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>change</t>
   </si>
   <si>
     <t xml:space="preserve">Wells drilled, completed, and drilled but uncompleted (DUC) inventory </t>
@@ -187,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -277,6 +289,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -354,7 +375,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -416,15 +437,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="5">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Body: normal cell" xfId="2"/>
@@ -727,10 +745,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF44"/>
+  <dimension ref="A1:AF46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH40" sqref="AH40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +790,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -806,7 +824,7 @@
       <c r="AE1" s="2"/>
       <c r="AF1" s="2"/>
     </row>
-    <row r="2" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -844,53 +862,53 @@
       <c r="A3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
       <c r="M3" s="23"/>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
       <c r="Q3" s="23"/>
-      <c r="R3" s="30" t="s">
+      <c r="R3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
       <c r="U3" s="23"/>
-      <c r="V3" s="30" t="s">
+      <c r="V3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
       <c r="Y3" s="23"/>
-      <c r="Z3" s="30" t="s">
+      <c r="Z3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
+      <c r="AA3" s="32"/>
+      <c r="AB3" s="32"/>
       <c r="AC3" s="23"/>
-      <c r="AD3" s="30" t="s">
+      <c r="AD3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="30"/>
-      <c r="AF3" s="30"/>
+      <c r="AE3" s="32"/>
+      <c r="AF3" s="32"/>
     </row>
     <row r="4" spans="1:32" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -997,7 +1015,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="19">
-        <v>929</v>
+        <v>932</v>
       </c>
       <c r="I5" s="17"/>
       <c r="J5" s="22" t="s">
@@ -1017,7 +1035,7 @@
         <v>10</v>
       </c>
       <c r="P5" s="19">
-        <v>863</v>
+        <v>872</v>
       </c>
       <c r="Q5" s="15"/>
       <c r="R5" s="22" t="s">
@@ -1037,7 +1055,7 @@
         <v>10</v>
       </c>
       <c r="X5" s="19">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="Y5" s="15"/>
       <c r="Z5" s="22" t="s">
@@ -1057,14 +1075,14 @@
         <v>10</v>
       </c>
       <c r="AF5" s="19">
-        <v>3709</v>
+        <v>3722</v>
       </c>
     </row>
     <row r="6" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>41640</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="25">
         <v>179</v>
       </c>
       <c r="C6" s="24">
@@ -1074,17 +1092,17 @@
         <v>605</v>
       </c>
       <c r="E6" s="19"/>
-      <c r="F6" s="24">
-        <v>335</v>
+      <c r="F6" s="25">
+        <v>336</v>
       </c>
       <c r="G6" s="24">
         <v>334</v>
       </c>
       <c r="H6" s="19">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="I6" s="19"/>
-      <c r="J6" s="24">
+      <c r="J6" s="25">
         <v>29</v>
       </c>
       <c r="K6" s="24">
@@ -1094,17 +1112,17 @@
         <v>112</v>
       </c>
       <c r="M6" s="19"/>
-      <c r="N6" s="24">
-        <v>106</v>
+      <c r="N6" s="25">
+        <v>111</v>
       </c>
       <c r="O6" s="24">
         <v>90</v>
       </c>
       <c r="P6" s="19">
-        <v>879</v>
+        <v>893</v>
       </c>
       <c r="Q6" s="19"/>
-      <c r="R6" s="24">
+      <c r="R6" s="25">
         <v>164</v>
       </c>
       <c r="S6" s="24">
@@ -1114,17 +1132,17 @@
         <v>429</v>
       </c>
       <c r="U6" s="19"/>
-      <c r="V6" s="24">
-        <v>580</v>
+      <c r="V6" s="25">
+        <v>581</v>
       </c>
       <c r="W6" s="24">
         <v>582</v>
       </c>
       <c r="X6" s="19">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="Y6" s="19"/>
-      <c r="Z6" s="24">
+      <c r="Z6" s="25">
         <v>26</v>
       </c>
       <c r="AA6" s="24">
@@ -1134,21 +1152,21 @@
         <v>210</v>
       </c>
       <c r="AC6" s="19"/>
-      <c r="AD6" s="24">
-        <v>1419</v>
+      <c r="AD6" s="25">
+        <v>1426</v>
       </c>
       <c r="AE6" s="24">
         <v>1346</v>
       </c>
       <c r="AF6" s="19">
-        <v>3782</v>
+        <v>3802</v>
       </c>
     </row>
     <row r="7" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>41671</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="25">
         <v>210</v>
       </c>
       <c r="C7" s="24">
@@ -1158,17 +1176,17 @@
         <v>657</v>
       </c>
       <c r="E7" s="19"/>
-      <c r="F7" s="24">
-        <v>374</v>
+      <c r="F7" s="25">
+        <v>373</v>
       </c>
       <c r="G7" s="24">
         <v>313</v>
       </c>
       <c r="H7" s="19">
-        <v>991</v>
+        <v>994</v>
       </c>
       <c r="I7" s="19"/>
-      <c r="J7" s="24">
+      <c r="J7" s="25">
         <v>47</v>
       </c>
       <c r="K7" s="24">
@@ -1178,38 +1196,38 @@
         <v>123</v>
       </c>
       <c r="M7" s="19"/>
-      <c r="N7" s="24">
-        <v>120</v>
+      <c r="N7" s="25">
+        <v>119</v>
       </c>
       <c r="O7" s="24">
         <v>99</v>
       </c>
       <c r="P7" s="19">
-        <v>900</v>
+        <v>913</v>
       </c>
       <c r="Q7" s="19"/>
-      <c r="R7" s="24">
-        <v>169</v>
+      <c r="R7" s="25">
+        <v>170</v>
       </c>
       <c r="S7" s="24">
         <v>125</v>
       </c>
       <c r="T7" s="19">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="U7" s="19"/>
-      <c r="V7" s="24">
+      <c r="V7" s="25">
         <v>578</v>
       </c>
       <c r="W7" s="24">
         <v>512</v>
       </c>
       <c r="X7" s="19">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="Y7" s="19"/>
-      <c r="Z7" s="24">
-        <v>29.000000000000004</v>
+      <c r="Z7" s="25">
+        <v>29</v>
       </c>
       <c r="AA7" s="24">
         <v>29</v>
@@ -1218,21 +1236,21 @@
         <v>210</v>
       </c>
       <c r="AC7" s="19"/>
-      <c r="AD7" s="24">
-        <v>1527</v>
+      <c r="AD7" s="25">
+        <v>1526</v>
       </c>
       <c r="AE7" s="24">
         <v>1272</v>
       </c>
       <c r="AF7" s="19">
-        <v>4037</v>
+        <v>4056</v>
       </c>
     </row>
     <row r="8" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>41699</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="25">
         <v>223</v>
       </c>
       <c r="C8" s="24">
@@ -1242,17 +1260,17 @@
         <v>662</v>
       </c>
       <c r="E8" s="19"/>
-      <c r="F8" s="24">
-        <v>352</v>
+      <c r="F8" s="25">
+        <v>353</v>
       </c>
       <c r="G8" s="24">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H8" s="19">
-        <v>960</v>
+        <v>963</v>
       </c>
       <c r="I8" s="19"/>
-      <c r="J8" s="24">
+      <c r="J8" s="25">
         <v>43</v>
       </c>
       <c r="K8" s="24">
@@ -1262,37 +1280,37 @@
         <v>120</v>
       </c>
       <c r="M8" s="19"/>
-      <c r="N8" s="24">
-        <v>92</v>
+      <c r="N8" s="25">
+        <v>83</v>
       </c>
       <c r="O8" s="24">
         <v>149</v>
       </c>
       <c r="P8" s="19">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="Q8" s="19"/>
-      <c r="R8" s="24">
-        <v>164</v>
+      <c r="R8" s="25">
+        <v>165</v>
       </c>
       <c r="S8" s="24">
         <v>186</v>
       </c>
       <c r="T8" s="19">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="U8" s="19"/>
-      <c r="V8" s="24">
+      <c r="V8" s="25">
         <v>595</v>
       </c>
       <c r="W8" s="24">
         <v>613</v>
       </c>
       <c r="X8" s="19">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="Y8" s="19"/>
-      <c r="Z8" s="24">
+      <c r="Z8" s="25">
         <v>31</v>
       </c>
       <c r="AA8" s="24">
@@ -1302,21 +1320,21 @@
         <v>212</v>
       </c>
       <c r="AC8" s="19"/>
-      <c r="AD8" s="24">
-        <v>1500</v>
+      <c r="AD8" s="25">
+        <v>1493</v>
       </c>
       <c r="AE8" s="24">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="AF8" s="19">
-        <v>3913</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="9" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>41730</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="25">
         <v>217</v>
       </c>
       <c r="C9" s="24">
@@ -1326,17 +1344,17 @@
         <v>672</v>
       </c>
       <c r="E9" s="19"/>
-      <c r="F9" s="24">
+      <c r="F9" s="25">
         <v>413</v>
       </c>
       <c r="G9" s="24">
         <v>335</v>
       </c>
       <c r="H9" s="19">
-        <v>1038</v>
+        <v>1041</v>
       </c>
       <c r="I9" s="19"/>
-      <c r="J9" s="24">
+      <c r="J9" s="25">
         <v>48</v>
       </c>
       <c r="K9" s="24">
@@ -1346,38 +1364,38 @@
         <v>114</v>
       </c>
       <c r="M9" s="19"/>
-      <c r="N9" s="24">
-        <v>163</v>
+      <c r="N9" s="25">
+        <v>151</v>
       </c>
       <c r="O9" s="24">
         <v>133</v>
       </c>
       <c r="P9" s="19">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="Q9" s="19"/>
-      <c r="R9" s="24">
-        <v>194</v>
+      <c r="R9" s="25">
+        <v>193</v>
       </c>
       <c r="S9" s="24">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="T9" s="19">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="U9" s="19"/>
-      <c r="V9" s="24">
-        <v>652</v>
+      <c r="V9" s="25">
+        <v>653</v>
       </c>
       <c r="W9" s="24">
         <v>623</v>
       </c>
       <c r="X9" s="19">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="Y9" s="19"/>
-      <c r="Z9" s="24">
-        <v>38.999999999999993</v>
+      <c r="Z9" s="25">
+        <v>39</v>
       </c>
       <c r="AA9" s="24">
         <v>36</v>
@@ -1386,41 +1404,41 @@
         <v>215</v>
       </c>
       <c r="AC9" s="19"/>
-      <c r="AD9" s="24">
-        <v>1726</v>
+      <c r="AD9" s="25">
+        <v>1714</v>
       </c>
       <c r="AE9" s="24">
-        <v>1579</v>
+        <v>1581</v>
       </c>
       <c r="AF9" s="19">
-        <v>4060</v>
+        <v>4057</v>
       </c>
     </row>
     <row r="10" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>41760</v>
       </c>
-      <c r="B10" s="24">
-        <v>224.99999999999997</v>
+      <c r="B10" s="25">
+        <v>226</v>
       </c>
       <c r="C10" s="24">
         <v>208</v>
       </c>
       <c r="D10" s="19">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="E10" s="19"/>
-      <c r="F10" s="24">
-        <v>370</v>
+      <c r="F10" s="25">
+        <v>368</v>
       </c>
       <c r="G10" s="24">
         <v>347</v>
       </c>
       <c r="H10" s="19">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="I10" s="19"/>
-      <c r="J10" s="24">
+      <c r="J10" s="25">
         <v>32</v>
       </c>
       <c r="K10" s="24">
@@ -1430,72 +1448,72 @@
         <v>107</v>
       </c>
       <c r="M10" s="19"/>
-      <c r="N10" s="24">
-        <v>136</v>
+      <c r="N10" s="25">
+        <v>131</v>
       </c>
       <c r="O10" s="24">
         <v>152</v>
       </c>
       <c r="P10" s="19">
-        <v>857</v>
+        <v>844</v>
       </c>
       <c r="Q10" s="19"/>
-      <c r="R10" s="24">
-        <v>201</v>
+      <c r="R10" s="25">
+        <v>200</v>
       </c>
       <c r="S10" s="24">
         <v>175</v>
       </c>
       <c r="T10" s="19">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="U10" s="19"/>
-      <c r="V10" s="24">
-        <v>636</v>
+      <c r="V10" s="25">
+        <v>635</v>
       </c>
       <c r="W10" s="24">
         <v>622</v>
       </c>
       <c r="X10" s="19">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="Y10" s="19"/>
-      <c r="Z10" s="24">
-        <v>40</v>
+      <c r="Z10" s="25">
+        <v>41</v>
       </c>
       <c r="AA10" s="24">
         <v>55</v>
       </c>
       <c r="AB10" s="19">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AC10" s="19"/>
-      <c r="AD10" s="24">
-        <v>1640</v>
+      <c r="AD10" s="25">
+        <v>1633</v>
       </c>
       <c r="AE10" s="24">
         <v>1598</v>
       </c>
       <c r="AF10" s="19">
-        <v>4102</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="11" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>41791</v>
       </c>
-      <c r="B11" s="24">
-        <v>234.00000000000003</v>
+      <c r="B11" s="25">
+        <v>234</v>
       </c>
       <c r="C11" s="24">
         <v>225</v>
       </c>
       <c r="D11" s="19">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="E11" s="19"/>
-      <c r="F11" s="24">
-        <v>363</v>
+      <c r="F11" s="25">
+        <v>362</v>
       </c>
       <c r="G11" s="24">
         <v>351</v>
@@ -1504,7 +1522,7 @@
         <v>1073</v>
       </c>
       <c r="I11" s="19"/>
-      <c r="J11" s="24">
+      <c r="J11" s="25">
         <v>37</v>
       </c>
       <c r="K11" s="24">
@@ -1514,18 +1532,18 @@
         <v>105</v>
       </c>
       <c r="M11" s="19"/>
-      <c r="N11" s="24">
-        <v>119.00000000000001</v>
+      <c r="N11" s="25">
+        <v>111</v>
       </c>
       <c r="O11" s="24">
         <v>158</v>
       </c>
       <c r="P11" s="19">
-        <v>818</v>
+        <v>797</v>
       </c>
       <c r="Q11" s="19"/>
-      <c r="R11" s="24">
-        <v>197</v>
+      <c r="R11" s="25">
+        <v>199</v>
       </c>
       <c r="S11" s="24">
         <v>184</v>
@@ -1534,34 +1552,34 @@
         <v>493</v>
       </c>
       <c r="U11" s="19"/>
-      <c r="V11" s="24">
-        <v>662</v>
+      <c r="V11" s="25">
+        <v>661</v>
       </c>
       <c r="W11" s="24">
         <v>608</v>
       </c>
       <c r="X11" s="19">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="Y11" s="19"/>
-      <c r="Z11" s="24">
+      <c r="Z11" s="25">
         <v>49</v>
       </c>
       <c r="AA11" s="24">
         <v>43</v>
       </c>
       <c r="AB11" s="19">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AC11" s="19"/>
-      <c r="AD11" s="24">
-        <v>1661</v>
+      <c r="AD11" s="25">
+        <v>1653</v>
       </c>
       <c r="AE11" s="24">
         <v>1608</v>
       </c>
       <c r="AF11" s="19">
-        <v>4155</v>
+        <v>4137</v>
       </c>
     </row>
     <row r="12" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1569,83 +1587,83 @@
         <v>41821</v>
       </c>
       <c r="B12" s="25">
-        <v>252.47524752475246</v>
+        <v>251</v>
       </c>
       <c r="C12" s="24">
         <v>243</v>
       </c>
       <c r="D12" s="19">
-        <v>707.47524752475249</v>
+        <v>707</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25">
-        <v>357.37008959338385</v>
+        <v>350</v>
       </c>
       <c r="G12" s="24">
         <v>328</v>
       </c>
       <c r="H12" s="19">
-        <v>1102.3700895933839</v>
+        <v>1095</v>
       </c>
       <c r="I12" s="19"/>
       <c r="J12" s="25">
-        <v>43.80952380952381</v>
+        <v>34</v>
       </c>
       <c r="K12" s="24">
         <v>50</v>
       </c>
       <c r="L12" s="19">
-        <v>98.809523809523796</v>
+        <v>89</v>
       </c>
       <c r="M12" s="19"/>
       <c r="N12" s="25">
-        <v>143.35913312693501</v>
+        <v>74</v>
       </c>
       <c r="O12" s="24">
         <v>126</v>
       </c>
       <c r="P12" s="19">
-        <v>835.35913312693503</v>
+        <v>745</v>
       </c>
       <c r="Q12" s="19"/>
       <c r="R12" s="25">
-        <v>200.60240963855421</v>
+        <v>194</v>
       </c>
       <c r="S12" s="24">
         <v>179</v>
       </c>
       <c r="T12" s="19">
-        <v>514.60240963855426</v>
+        <v>508</v>
       </c>
       <c r="U12" s="19"/>
       <c r="V12" s="25">
-        <v>664.42674961119747</v>
+        <v>604</v>
       </c>
       <c r="W12" s="24">
         <v>600</v>
       </c>
       <c r="X12" s="19">
-        <v>826.42674961119747</v>
+        <v>767</v>
       </c>
       <c r="Y12" s="19"/>
       <c r="Z12" s="25">
-        <v>46.096153846153847</v>
+        <v>50</v>
       </c>
       <c r="AA12" s="24">
         <v>46</v>
       </c>
       <c r="AB12" s="19">
-        <v>206.09615384615384</v>
+        <v>211</v>
       </c>
       <c r="AC12" s="19"/>
       <c r="AD12" s="25">
-        <v>1708.1393071505006</v>
+        <v>1557</v>
       </c>
       <c r="AE12" s="24">
         <v>1572</v>
       </c>
       <c r="AF12" s="19">
-        <v>4291.1393071505008</v>
+        <v>4122</v>
       </c>
     </row>
     <row r="13" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1653,83 +1671,83 @@
         <v>41852</v>
       </c>
       <c r="B13" s="25">
-        <v>253.46534653465346</v>
+        <v>224</v>
       </c>
       <c r="C13" s="24">
         <v>207</v>
       </c>
       <c r="D13" s="19">
-        <v>753.94059405940595</v>
+        <v>724</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25">
-        <v>372.85182632667124</v>
+        <v>347</v>
       </c>
       <c r="G13" s="24">
         <v>364</v>
       </c>
       <c r="H13" s="19">
-        <v>1111.2219159200552</v>
+        <v>1078</v>
       </c>
       <c r="I13" s="19"/>
       <c r="J13" s="25">
-        <v>38.095238095238095</v>
+        <v>36</v>
       </c>
       <c r="K13" s="24">
         <v>33</v>
       </c>
       <c r="L13" s="19">
-        <v>103.9047619047619</v>
+        <v>92</v>
       </c>
       <c r="M13" s="19"/>
       <c r="N13" s="25">
-        <v>111.1764705882353</v>
+        <v>84</v>
       </c>
       <c r="O13" s="24">
         <v>140</v>
       </c>
       <c r="P13" s="19">
-        <v>806.53560371517028</v>
+        <v>689</v>
       </c>
       <c r="Q13" s="19"/>
       <c r="R13" s="25">
-        <v>188.34337349397589</v>
+        <v>205</v>
       </c>
       <c r="S13" s="24">
         <v>183</v>
       </c>
       <c r="T13" s="19">
-        <v>519.9457831325301</v>
+        <v>530</v>
       </c>
       <c r="U13" s="19"/>
       <c r="V13" s="25">
-        <v>621.68584758942461</v>
+        <v>648</v>
       </c>
       <c r="W13" s="24">
         <v>573</v>
       </c>
       <c r="X13" s="19">
-        <v>875.11259720062208</v>
+        <v>842</v>
       </c>
       <c r="Y13" s="19"/>
       <c r="Z13" s="25">
-        <v>37.96153846153846</v>
+        <v>61</v>
       </c>
       <c r="AA13" s="24">
         <v>52</v>
       </c>
       <c r="AB13" s="19">
-        <v>192.05769230769229</v>
+        <v>220</v>
       </c>
       <c r="AC13" s="19"/>
       <c r="AD13" s="25">
-        <v>1623.5796410897372</v>
+        <v>1605</v>
       </c>
       <c r="AE13" s="24">
         <v>1552</v>
       </c>
       <c r="AF13" s="19">
-        <v>4362.7189482402382</v>
+        <v>4175</v>
       </c>
     </row>
     <row r="14" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1737,83 +1755,83 @@
         <v>41883</v>
       </c>
       <c r="B14" s="25">
-        <v>239.60396039603961</v>
+        <v>248</v>
       </c>
       <c r="C14" s="24">
         <v>232</v>
       </c>
       <c r="D14" s="19">
-        <v>761.54455445544556</v>
+        <v>740</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25">
-        <v>380.59269469331497</v>
+        <v>376</v>
       </c>
       <c r="G14" s="24">
         <v>335</v>
       </c>
       <c r="H14" s="19">
-        <v>1156.8146106133702</v>
+        <v>1119</v>
       </c>
       <c r="I14" s="19"/>
       <c r="J14" s="25">
-        <v>42.857142857142854</v>
+        <v>34</v>
       </c>
       <c r="K14" s="24">
         <v>37</v>
       </c>
       <c r="L14" s="19">
-        <v>109.76190476190476</v>
+        <v>89</v>
       </c>
       <c r="M14" s="19"/>
       <c r="N14" s="25">
-        <v>130.6811145510836</v>
+        <v>113</v>
       </c>
       <c r="O14" s="24">
         <v>171</v>
       </c>
       <c r="P14" s="19">
-        <v>766.21671826625391</v>
+        <v>631</v>
       </c>
       <c r="Q14" s="19"/>
       <c r="R14" s="25">
-        <v>213.97590361445782</v>
+        <v>209</v>
       </c>
       <c r="S14" s="24">
         <v>207</v>
       </c>
       <c r="T14" s="19">
-        <v>526.92168674698792</v>
+        <v>532</v>
       </c>
       <c r="U14" s="19"/>
       <c r="V14" s="25">
-        <v>663.45536547433903</v>
+        <v>659</v>
       </c>
       <c r="W14" s="24">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="X14" s="19">
-        <v>951.56796267496111</v>
+        <v>913</v>
       </c>
       <c r="Y14" s="19"/>
       <c r="Z14" s="25">
-        <v>52.42307692307692</v>
+        <v>63</v>
       </c>
       <c r="AA14" s="24">
         <v>46</v>
       </c>
       <c r="AB14" s="19">
-        <v>198.48076923076923</v>
+        <v>237</v>
       </c>
       <c r="AC14" s="19"/>
       <c r="AD14" s="25">
-        <v>1723.5892585094548</v>
+        <v>1702</v>
       </c>
       <c r="AE14" s="24">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="AF14" s="19">
-        <v>4471.3082067496925</v>
+        <v>4261</v>
       </c>
     </row>
     <row r="15" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1821,83 +1839,83 @@
         <v>41913</v>
       </c>
       <c r="B15" s="25">
-        <v>187.12871287128712</v>
+        <v>193</v>
       </c>
       <c r="C15" s="24">
         <v>243</v>
       </c>
       <c r="D15" s="19">
-        <v>705.67326732673268</v>
+        <v>690</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="25">
-        <v>403.81529979324603</v>
+        <v>404</v>
       </c>
       <c r="G15" s="24">
         <v>415</v>
       </c>
       <c r="H15" s="19">
-        <v>1145.6299104066161</v>
+        <v>1108</v>
       </c>
       <c r="I15" s="19"/>
       <c r="J15" s="25">
-        <v>49.523809523809518</v>
+        <v>52</v>
       </c>
       <c r="K15" s="24">
         <v>32</v>
       </c>
       <c r="L15" s="19">
-        <v>127.28571428571428</v>
+        <v>109</v>
       </c>
       <c r="M15" s="19"/>
       <c r="N15" s="25">
-        <v>144.33436532507741</v>
+        <v>154</v>
       </c>
       <c r="O15" s="24">
         <v>156</v>
       </c>
       <c r="P15" s="19">
-        <v>754.55108359133135</v>
+        <v>629</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="25">
-        <v>188.34337349397589</v>
+        <v>189</v>
       </c>
       <c r="S15" s="24">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="T15" s="19">
-        <v>539.26506024096375</v>
+        <v>544</v>
       </c>
       <c r="U15" s="19"/>
       <c r="V15" s="25">
-        <v>682.88304821150859</v>
+        <v>695</v>
       </c>
       <c r="W15" s="24">
         <v>660</v>
       </c>
       <c r="X15" s="19">
-        <v>974.4510108864697</v>
+        <v>948</v>
       </c>
       <c r="Y15" s="19"/>
       <c r="Z15" s="25">
-        <v>43.38461538461538</v>
+        <v>42</v>
       </c>
       <c r="AA15" s="24">
         <v>37</v>
       </c>
       <c r="AB15" s="19">
-        <v>204.86538461538461</v>
+        <v>242</v>
       </c>
       <c r="AC15" s="19"/>
       <c r="AD15" s="25">
-        <v>1699.4132246035201</v>
+        <v>1729</v>
       </c>
       <c r="AE15" s="24">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="AF15" s="19">
-        <v>4451.7214313532131</v>
+        <v>4270</v>
       </c>
     </row>
     <row r="16" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1905,83 +1923,83 @@
         <v>41944</v>
       </c>
       <c r="B16" s="25">
-        <v>203.96039603960395</v>
+        <v>210</v>
       </c>
       <c r="C16" s="24">
         <v>202</v>
       </c>
       <c r="D16" s="19">
-        <v>707.63366336633658</v>
+        <v>698</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="25">
-        <v>317.37560303239144</v>
+        <v>317</v>
       </c>
       <c r="G16" s="24">
         <v>398</v>
       </c>
       <c r="H16" s="19">
-        <v>1065.0055134390075</v>
+        <v>1027</v>
       </c>
       <c r="I16" s="19"/>
       <c r="J16" s="25">
-        <v>36.19047619047619</v>
+        <v>38</v>
       </c>
       <c r="K16" s="24">
         <v>36</v>
       </c>
       <c r="L16" s="19">
-        <v>127.47619047619048</v>
+        <v>111</v>
       </c>
       <c r="M16" s="19"/>
       <c r="N16" s="25">
-        <v>102.39938080495357</v>
+        <v>109</v>
       </c>
       <c r="O16" s="24">
         <v>137</v>
       </c>
       <c r="P16" s="19">
-        <v>719.95046439628493</v>
+        <v>601</v>
       </c>
       <c r="Q16" s="19"/>
       <c r="R16" s="25">
-        <v>157.13855421686745</v>
+        <v>158</v>
       </c>
       <c r="S16" s="24">
         <v>166</v>
       </c>
       <c r="T16" s="19">
-        <v>530.40361445783117</v>
+        <v>536</v>
       </c>
       <c r="U16" s="19"/>
       <c r="V16" s="25">
-        <v>548.83203732503887</v>
+        <v>558</v>
       </c>
       <c r="W16" s="24">
         <v>569</v>
       </c>
       <c r="X16" s="19">
-        <v>954.28304821150869</v>
+        <v>937</v>
       </c>
       <c r="Y16" s="19"/>
       <c r="Z16" s="25">
-        <v>37.057692307692307</v>
+        <v>36</v>
       </c>
       <c r="AA16" s="24">
         <v>37</v>
       </c>
       <c r="AB16" s="19">
-        <v>204.92307692307691</v>
+        <v>241</v>
       </c>
       <c r="AC16" s="19"/>
       <c r="AD16" s="25">
-        <v>1402.9541399170237</v>
+        <v>1426</v>
       </c>
       <c r="AE16" s="24">
         <v>1545</v>
       </c>
       <c r="AF16" s="19">
-        <v>4309.675571270237</v>
+        <v>4151</v>
       </c>
     </row>
     <row r="17" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1989,83 +2007,83 @@
         <v>41974</v>
       </c>
       <c r="B17" s="25">
-        <v>227.72277227722773</v>
+        <v>235</v>
       </c>
       <c r="C17" s="24">
         <v>194</v>
       </c>
       <c r="D17" s="19">
-        <v>741.35643564356428</v>
+        <v>739</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="25">
-        <v>353.49965541006202</v>
+        <v>354</v>
       </c>
       <c r="G17" s="24">
         <v>386</v>
       </c>
       <c r="H17" s="19">
-        <v>1032.5051688490694</v>
+        <v>995</v>
       </c>
       <c r="I17" s="19"/>
       <c r="J17" s="25">
-        <v>47.61904761904762</v>
+        <v>50</v>
       </c>
       <c r="K17" s="24">
         <v>38</v>
       </c>
       <c r="L17" s="19">
-        <v>137.0952380952381</v>
+        <v>123</v>
       </c>
       <c r="M17" s="19"/>
       <c r="N17" s="25">
-        <v>130.6811145510836</v>
+        <v>140</v>
       </c>
       <c r="O17" s="24">
         <v>144</v>
       </c>
       <c r="P17" s="19">
-        <v>706.63157894736855</v>
+        <v>597</v>
       </c>
       <c r="Q17" s="19"/>
       <c r="R17" s="25">
-        <v>206.17469879518072</v>
+        <v>207</v>
       </c>
       <c r="S17" s="24">
         <v>188</v>
       </c>
       <c r="T17" s="19">
-        <v>548.57831325301186</v>
+        <v>555</v>
       </c>
       <c r="U17" s="19"/>
       <c r="V17" s="25">
-        <v>623.62861586314148</v>
+        <v>634</v>
       </c>
       <c r="W17" s="24">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="X17" s="19">
-        <v>1010.9116640746502</v>
+        <v>1001</v>
       </c>
       <c r="Y17" s="19"/>
       <c r="Z17" s="25">
-        <v>49.71153846153846</v>
+        <v>48</v>
       </c>
       <c r="AA17" s="24">
         <v>35</v>
       </c>
       <c r="AB17" s="19">
-        <v>219.63461538461536</v>
+        <v>254</v>
       </c>
       <c r="AC17" s="19"/>
       <c r="AD17" s="25">
-        <v>1639.0374429772814</v>
+        <v>1668</v>
       </c>
       <c r="AE17" s="24">
-        <v>1552</v>
+        <v>1555</v>
       </c>
       <c r="AF17" s="19">
-        <v>4396.713014247518</v>
+        <v>4264</v>
       </c>
     </row>
     <row r="18" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2073,83 +2091,83 @@
         <v>42005</v>
       </c>
       <c r="B18" s="25">
-        <v>195.04950495049505</v>
+        <v>201</v>
       </c>
       <c r="C18" s="24">
         <v>193</v>
       </c>
       <c r="D18" s="19">
-        <v>743.4059405940593</v>
+        <v>747</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="25">
-        <v>430.90833907649898</v>
+        <v>431</v>
       </c>
       <c r="G18" s="24">
         <v>349</v>
       </c>
       <c r="H18" s="19">
-        <v>1114.4135079255684</v>
+        <v>1077</v>
       </c>
       <c r="I18" s="19"/>
       <c r="J18" s="25">
-        <v>36.19047619047619</v>
+        <v>38</v>
       </c>
       <c r="K18" s="24">
         <v>48</v>
       </c>
       <c r="L18" s="19">
-        <v>125.28571428571428</v>
+        <v>113</v>
       </c>
       <c r="M18" s="19"/>
       <c r="N18" s="25">
-        <v>137.5077399380805</v>
+        <v>147</v>
       </c>
       <c r="O18" s="24">
         <v>141</v>
       </c>
       <c r="P18" s="19">
-        <v>703.13931888544903</v>
+        <v>603</v>
       </c>
       <c r="Q18" s="19"/>
       <c r="R18" s="25">
-        <v>195.0301204819277</v>
+        <v>196</v>
       </c>
       <c r="S18" s="24">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="T18" s="19">
-        <v>583.60843373493958</v>
+        <v>590</v>
       </c>
       <c r="U18" s="19"/>
       <c r="V18" s="25">
-        <v>575.05940902021769</v>
+        <v>585</v>
       </c>
       <c r="W18" s="24">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="X18" s="19">
-        <v>1117.9710730948677</v>
+        <v>1116</v>
       </c>
       <c r="Y18" s="19"/>
       <c r="Z18" s="25">
-        <v>52.42307692307692</v>
+        <v>50</v>
       </c>
       <c r="AA18" s="24">
         <v>32</v>
       </c>
       <c r="AB18" s="19">
-        <v>240.05769230769226</v>
+        <v>272</v>
       </c>
       <c r="AC18" s="19"/>
       <c r="AD18" s="25">
-        <v>1622.1686665807729</v>
+        <v>1648</v>
       </c>
       <c r="AE18" s="24">
-        <v>1391</v>
+        <v>1394</v>
       </c>
       <c r="AF18" s="19">
-        <v>4627.8816808282909</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="19" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2157,83 +2175,83 @@
         <v>42036</v>
       </c>
       <c r="B19" s="25">
-        <v>225.74257425742573</v>
+        <v>233</v>
       </c>
       <c r="C19" s="24">
         <v>151</v>
       </c>
       <c r="D19" s="19">
-        <v>818.14851485148506</v>
+        <v>829</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="25">
-        <v>482.51412818745689</v>
+        <v>483</v>
       </c>
       <c r="G19" s="24">
         <v>260</v>
       </c>
       <c r="H19" s="19">
-        <v>1336.9276361130253</v>
+        <v>1300</v>
       </c>
       <c r="I19" s="19"/>
       <c r="J19" s="25">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K19" s="24">
         <v>39</v>
       </c>
       <c r="L19" s="19">
-        <v>126.28571428571428</v>
+        <v>116</v>
       </c>
       <c r="M19" s="19"/>
       <c r="N19" s="25">
-        <v>129.70588235294119</v>
+        <v>139</v>
       </c>
       <c r="O19" s="24">
         <v>87</v>
       </c>
       <c r="P19" s="19">
-        <v>745.84520123839025</v>
+        <v>655</v>
       </c>
       <c r="Q19" s="19"/>
       <c r="R19" s="25">
-        <v>203.9457831325301</v>
+        <v>204</v>
       </c>
       <c r="S19" s="24">
         <v>114</v>
       </c>
       <c r="T19" s="19">
-        <v>673.55421686746968</v>
+        <v>680</v>
       </c>
       <c r="U19" s="19"/>
       <c r="V19" s="25">
-        <v>505.11975116640747</v>
+        <v>514</v>
       </c>
       <c r="W19" s="24">
         <v>394</v>
       </c>
       <c r="X19" s="19">
-        <v>1229.0908242612752</v>
+        <v>1236</v>
       </c>
       <c r="Y19" s="19"/>
       <c r="Z19" s="25">
-        <v>45.192307692307693</v>
+        <v>43</v>
       </c>
       <c r="AA19" s="24">
         <v>28</v>
       </c>
       <c r="AB19" s="19">
-        <v>257.24999999999994</v>
+        <v>287</v>
       </c>
       <c r="AC19" s="19"/>
       <c r="AD19" s="25">
-        <v>1632.2204267890691</v>
+        <v>1658</v>
       </c>
       <c r="AE19" s="24">
         <v>1073</v>
       </c>
       <c r="AF19" s="19">
-        <v>5187.1021076173602</v>
+        <v>5103</v>
       </c>
     </row>
     <row r="20" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2241,83 +2259,83 @@
         <v>42064</v>
       </c>
       <c r="B20" s="25">
-        <v>183.16831683168317</v>
+        <v>189</v>
       </c>
       <c r="C20" s="24">
         <v>170</v>
       </c>
       <c r="D20" s="19">
-        <v>831.31683168316818</v>
+        <v>848</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="25">
-        <v>361.24052377670569</v>
+        <v>361</v>
       </c>
       <c r="G20" s="24">
         <v>283</v>
       </c>
       <c r="H20" s="19">
-        <v>1415.168159889731</v>
+        <v>1378</v>
       </c>
       <c r="I20" s="19"/>
       <c r="J20" s="25">
-        <v>42.857142857142854</v>
+        <v>45</v>
       </c>
       <c r="K20" s="24">
         <v>35</v>
       </c>
       <c r="L20" s="19">
-        <v>134.14285714285714</v>
+        <v>126</v>
       </c>
       <c r="M20" s="19"/>
       <c r="N20" s="25">
-        <v>133.60681114551085</v>
+        <v>143</v>
       </c>
       <c r="O20" s="24">
         <v>109</v>
       </c>
       <c r="P20" s="19">
-        <v>770.45201238390109</v>
+        <v>689</v>
       </c>
       <c r="Q20" s="19"/>
       <c r="R20" s="25">
-        <v>153.79518072289156</v>
+        <v>154</v>
       </c>
       <c r="S20" s="24">
         <v>168</v>
       </c>
       <c r="T20" s="19">
-        <v>659.34939759036126</v>
+        <v>666</v>
       </c>
       <c r="U20" s="19"/>
       <c r="V20" s="25">
-        <v>398.26749611197511</v>
+        <v>405</v>
       </c>
       <c r="W20" s="24">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="X20" s="19">
-        <v>1196.3583203732503</v>
+        <v>1202</v>
       </c>
       <c r="Y20" s="19"/>
       <c r="Z20" s="25">
-        <v>35.25</v>
+        <v>34</v>
       </c>
       <c r="AA20" s="24">
         <v>37</v>
       </c>
       <c r="AB20" s="19">
-        <v>255.49999999999994</v>
+        <v>284</v>
       </c>
       <c r="AC20" s="19"/>
       <c r="AD20" s="25">
-        <v>1308.1854714459091</v>
+        <v>1331</v>
       </c>
       <c r="AE20" s="24">
-        <v>1233</v>
+        <v>1241</v>
       </c>
       <c r="AF20" s="19">
-        <v>5262.2875790632697</v>
+        <v>5193</v>
       </c>
     </row>
     <row r="21" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2325,83 +2343,83 @@
         <v>42095</v>
       </c>
       <c r="B21" s="25">
-        <v>140.59405940594058</v>
+        <v>145</v>
       </c>
       <c r="C21" s="24">
         <v>127</v>
       </c>
       <c r="D21" s="19">
-        <v>844.91089108910876</v>
+        <v>866</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="25">
-        <v>264.47966919365956</v>
+        <v>265</v>
       </c>
       <c r="G21" s="24">
         <v>236</v>
       </c>
       <c r="H21" s="19">
-        <v>1443.6478290833907</v>
+        <v>1407</v>
       </c>
       <c r="I21" s="19"/>
       <c r="J21" s="25">
-        <v>26.666666666666664</v>
+        <v>28</v>
       </c>
       <c r="K21" s="24">
         <v>34</v>
       </c>
       <c r="L21" s="19">
-        <v>126.8095238095238</v>
+        <v>120</v>
       </c>
       <c r="M21" s="19"/>
       <c r="N21" s="25">
-        <v>105.32507739938082</v>
+        <v>113</v>
       </c>
       <c r="O21" s="24">
         <v>117</v>
       </c>
       <c r="P21" s="19">
-        <v>758.77708978328189</v>
+        <v>685</v>
       </c>
       <c r="Q21" s="19"/>
       <c r="R21" s="25">
-        <v>138.19277108433735</v>
+        <v>139</v>
       </c>
       <c r="S21" s="24">
         <v>140</v>
       </c>
       <c r="T21" s="19">
-        <v>657.54216867469859</v>
+        <v>665</v>
       </c>
       <c r="U21" s="19"/>
       <c r="V21" s="25">
-        <v>333.18475894245722</v>
+        <v>339</v>
       </c>
       <c r="W21" s="24">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="X21" s="19">
-        <v>1214.5430793157075</v>
+        <v>1222</v>
       </c>
       <c r="Y21" s="19"/>
       <c r="Z21" s="25">
-        <v>40.67307692307692</v>
+        <v>39</v>
       </c>
       <c r="AA21" s="24">
         <v>49</v>
       </c>
       <c r="AB21" s="19">
-        <v>247.17307692307685</v>
+        <v>274</v>
       </c>
       <c r="AC21" s="19"/>
       <c r="AD21" s="25">
-        <v>1049.1160796155191</v>
+        <v>1068</v>
       </c>
       <c r="AE21" s="24">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="AF21" s="19">
-        <v>5293.4036586787888</v>
+        <v>5239</v>
       </c>
     </row>
     <row r="22" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2409,83 +2427,83 @@
         <v>42125</v>
       </c>
       <c r="B22" s="25">
-        <v>117.82178217821782</v>
+        <v>121</v>
       </c>
       <c r="C22" s="24">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D22" s="19">
-        <v>824.73267326732662</v>
+        <v>848</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="25">
-        <v>238.67677463818055</v>
+        <v>239</v>
       </c>
       <c r="G22" s="24">
         <v>174</v>
       </c>
       <c r="H22" s="19">
-        <v>1508.3246037215713</v>
+        <v>1472</v>
       </c>
       <c r="I22" s="19"/>
       <c r="J22" s="25">
-        <v>26.666666666666664</v>
+        <v>28</v>
       </c>
       <c r="K22" s="24">
         <v>28</v>
       </c>
       <c r="L22" s="19">
-        <v>125.47619047619045</v>
+        <v>120</v>
       </c>
       <c r="M22" s="19"/>
       <c r="N22" s="25">
-        <v>115.07739938080496</v>
+        <v>123</v>
       </c>
       <c r="O22" s="24">
         <v>115</v>
       </c>
       <c r="P22" s="19">
-        <v>758.85448916408689</v>
+        <v>693</v>
       </c>
       <c r="Q22" s="19"/>
       <c r="R22" s="25">
-        <v>130.39156626506022</v>
+        <v>131</v>
       </c>
       <c r="S22" s="24">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="T22" s="19">
-        <v>670.93373493975878</v>
+        <v>678</v>
       </c>
       <c r="U22" s="19"/>
       <c r="V22" s="25">
-        <v>272.95894245723173</v>
+        <v>278</v>
       </c>
       <c r="W22" s="24">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="X22" s="19">
-        <v>1151.5020217729393</v>
+        <v>1162</v>
       </c>
       <c r="Y22" s="19"/>
       <c r="Z22" s="25">
-        <v>23.5</v>
+        <v>23</v>
       </c>
       <c r="AA22" s="24">
         <v>51</v>
       </c>
       <c r="AB22" s="19">
-        <v>219.67307692307685</v>
+        <v>246</v>
       </c>
       <c r="AC22" s="19"/>
       <c r="AD22" s="25">
-        <v>925.09313158616192</v>
+        <v>943</v>
       </c>
       <c r="AE22" s="24">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c r="AF22" s="19">
-        <v>5259.4967902649505</v>
+        <v>5219</v>
       </c>
     </row>
     <row r="23" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2493,83 +2511,83 @@
         <v>42156</v>
       </c>
       <c r="B23" s="25">
-        <v>104.95049504950495</v>
+        <v>108</v>
       </c>
       <c r="C23" s="24">
         <v>135</v>
       </c>
       <c r="D23" s="19">
-        <v>794.6831683168316</v>
+        <v>821</v>
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="25">
-        <v>225.77532736044108</v>
+        <v>226</v>
       </c>
       <c r="G23" s="24">
         <v>181</v>
       </c>
       <c r="H23" s="19">
-        <v>1553.0999310820123</v>
+        <v>1517</v>
       </c>
       <c r="I23" s="19"/>
       <c r="J23" s="25">
-        <v>21.904761904761905</v>
+        <v>23</v>
       </c>
       <c r="K23" s="24">
         <v>15</v>
       </c>
       <c r="L23" s="19">
-        <v>132.38095238095235</v>
+        <v>128</v>
       </c>
       <c r="M23" s="19"/>
       <c r="N23" s="25">
-        <v>93.622291021671842</v>
+        <v>100</v>
       </c>
       <c r="O23" s="24">
         <v>92</v>
       </c>
       <c r="P23" s="19">
-        <v>760.47678018575868</v>
+        <v>701</v>
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="25">
-        <v>129.27710843373492</v>
+        <v>130</v>
       </c>
       <c r="S23" s="24">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="T23" s="19">
-        <v>673.21084337349373</v>
+        <v>680</v>
       </c>
       <c r="U23" s="19"/>
       <c r="V23" s="25">
-        <v>303.07185069984445</v>
+        <v>308</v>
       </c>
       <c r="W23" s="24">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="X23" s="19">
-        <v>1105.5738724727837</v>
+        <v>1118</v>
       </c>
       <c r="Y23" s="19"/>
       <c r="Z23" s="25">
-        <v>28.923076923076923</v>
+        <v>28</v>
       </c>
       <c r="AA23" s="24">
         <v>46</v>
       </c>
       <c r="AB23" s="19">
-        <v>202.59615384615378</v>
+        <v>228</v>
       </c>
       <c r="AC23" s="19"/>
       <c r="AD23" s="25">
-        <v>907.52491139303606</v>
+        <v>923</v>
       </c>
       <c r="AE23" s="24">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c r="AF23" s="19">
-        <v>5222.0217016579863</v>
+        <v>5193</v>
       </c>
     </row>
     <row r="24" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2577,83 +2595,83 @@
         <v>42186</v>
       </c>
       <c r="B24" s="25">
-        <v>100.99009900990099</v>
+        <v>104</v>
       </c>
       <c r="C24" s="24">
         <v>124</v>
       </c>
       <c r="D24" s="19">
-        <v>771.67326732673257</v>
+        <v>801</v>
       </c>
       <c r="E24" s="25"/>
       <c r="F24" s="25">
-        <v>224.48518263266712</v>
+        <v>225</v>
       </c>
       <c r="G24" s="24">
         <v>212</v>
       </c>
       <c r="H24" s="19">
-        <v>1565.5851137146794</v>
+        <v>1530</v>
       </c>
       <c r="I24" s="19"/>
       <c r="J24" s="25">
-        <v>29.523809523809522</v>
+        <v>31</v>
       </c>
       <c r="K24" s="24">
         <v>20</v>
       </c>
       <c r="L24" s="19">
-        <v>141.90476190476187</v>
+        <v>139</v>
       </c>
       <c r="M24" s="19"/>
       <c r="N24" s="25">
-        <v>120.92879256965945</v>
+        <v>129</v>
       </c>
       <c r="O24" s="24">
         <v>101</v>
       </c>
       <c r="P24" s="19">
-        <v>780.40557275541812</v>
+        <v>729</v>
       </c>
       <c r="Q24" s="19"/>
       <c r="R24" s="25">
-        <v>124.81927710843372</v>
+        <v>125</v>
       </c>
       <c r="S24" s="24">
         <v>74</v>
       </c>
       <c r="T24" s="19">
-        <v>724.0301204819275</v>
+        <v>731</v>
       </c>
       <c r="U24" s="19"/>
       <c r="V24" s="25">
-        <v>296.27216174183513</v>
+        <v>301</v>
       </c>
       <c r="W24" s="24">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="X24" s="19">
-        <v>1043.8460342146188</v>
+        <v>1059</v>
       </c>
       <c r="Y24" s="19"/>
       <c r="Z24" s="25">
-        <v>24.403846153846153</v>
+        <v>23</v>
       </c>
       <c r="AA24" s="24">
         <v>35</v>
       </c>
       <c r="AB24" s="19">
-        <v>191.99999999999994</v>
+        <v>216</v>
       </c>
       <c r="AC24" s="19"/>
       <c r="AD24" s="25">
-        <v>921.42316874015205</v>
+        <v>938</v>
       </c>
       <c r="AE24" s="24">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="AF24" s="19">
-        <v>5219.4448703981379</v>
+        <v>5205</v>
       </c>
     </row>
     <row r="25" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2661,83 +2679,83 @@
         <v>42217</v>
       </c>
       <c r="B25" s="25">
-        <v>104.95049504950495</v>
+        <v>108</v>
       </c>
       <c r="C25" s="24">
         <v>101</v>
       </c>
       <c r="D25" s="19">
-        <v>775.62376237623755</v>
+        <v>808</v>
       </c>
       <c r="E25" s="25"/>
       <c r="F25" s="25">
-        <v>215.45416953824949</v>
+        <v>215</v>
       </c>
       <c r="G25" s="24">
         <v>246</v>
       </c>
       <c r="H25" s="19">
-        <v>1535.039283252929</v>
+        <v>1499</v>
       </c>
       <c r="I25" s="19"/>
       <c r="J25" s="25">
-        <v>31.428571428571427</v>
+        <v>33</v>
       </c>
       <c r="K25" s="24">
         <v>23</v>
       </c>
       <c r="L25" s="19">
-        <v>150.33333333333329</v>
+        <v>149</v>
       </c>
       <c r="M25" s="19"/>
       <c r="N25" s="25">
-        <v>87.77089783281734</v>
+        <v>94</v>
       </c>
       <c r="O25" s="24">
         <v>95</v>
       </c>
       <c r="P25" s="19">
-        <v>773.17647058823547</v>
+        <v>728</v>
       </c>
       <c r="Q25" s="19"/>
       <c r="R25" s="25">
-        <v>139.30722891566265</v>
+        <v>140</v>
       </c>
       <c r="S25" s="24">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="T25" s="19">
-        <v>749.33734939759017</v>
+        <v>754</v>
       </c>
       <c r="U25" s="19"/>
       <c r="V25" s="25">
-        <v>327.35645412130634</v>
+        <v>333</v>
       </c>
       <c r="W25" s="24">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="X25" s="19">
-        <v>1054.2024883359252</v>
+        <v>1070</v>
       </c>
       <c r="Y25" s="19"/>
       <c r="Z25" s="25">
-        <v>22.596153846153847</v>
+        <v>22</v>
       </c>
       <c r="AA25" s="24">
         <v>40</v>
       </c>
       <c r="AB25" s="19">
-        <v>174.59615384615378</v>
+        <v>198</v>
       </c>
       <c r="AC25" s="19"/>
       <c r="AD25" s="25">
-        <v>928.86397073226613</v>
+        <v>945</v>
       </c>
       <c r="AE25" s="24">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="AF25" s="19">
-        <v>5212.3088411304043</v>
+        <v>5206</v>
       </c>
     </row>
     <row r="26" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2745,83 +2763,83 @@
         <v>42248</v>
       </c>
       <c r="B26" s="25">
-        <v>96.039603960396036</v>
+        <v>99</v>
       </c>
       <c r="C26" s="24">
         <v>92</v>
       </c>
       <c r="D26" s="19">
-        <v>779.66336633663354</v>
+        <v>815</v>
       </c>
       <c r="E26" s="25"/>
       <c r="F26" s="25">
-        <v>203.84286698828393</v>
+        <v>204</v>
       </c>
       <c r="G26" s="24">
         <v>225</v>
       </c>
       <c r="H26" s="19">
-        <v>1513.8821502412129</v>
+        <v>1478</v>
       </c>
       <c r="I26" s="19"/>
       <c r="J26" s="25">
-        <v>31.428571428571427</v>
+        <v>33</v>
       </c>
       <c r="K26" s="24">
         <v>22</v>
       </c>
       <c r="L26" s="19">
-        <v>159.7619047619047</v>
+        <v>160</v>
       </c>
       <c r="M26" s="19"/>
       <c r="N26" s="25">
-        <v>83.869969040247682</v>
+        <v>90</v>
       </c>
       <c r="O26" s="24">
         <v>112</v>
       </c>
       <c r="P26" s="19">
-        <v>745.0464396284832</v>
+        <v>706</v>
       </c>
       <c r="Q26" s="19"/>
       <c r="R26" s="25">
-        <v>122.59036144578313</v>
+        <v>123</v>
       </c>
       <c r="S26" s="24">
         <v>97</v>
       </c>
       <c r="T26" s="19">
-        <v>774.92771084337335</v>
+        <v>780</v>
       </c>
       <c r="U26" s="19"/>
       <c r="V26" s="25">
-        <v>322.49953343701401</v>
+        <v>328</v>
       </c>
       <c r="W26" s="24">
         <v>280</v>
       </c>
       <c r="X26" s="19">
-        <v>1096.7020217729391</v>
+        <v>1118</v>
       </c>
       <c r="Y26" s="19"/>
       <c r="Z26" s="25">
-        <v>25.307692307692307</v>
+        <v>24</v>
       </c>
       <c r="AA26" s="24">
         <v>26</v>
       </c>
       <c r="AB26" s="19">
-        <v>173.90384615384608</v>
+        <v>196</v>
       </c>
       <c r="AC26" s="19"/>
       <c r="AD26" s="25">
-        <v>885.57859860798851</v>
+        <v>901</v>
       </c>
       <c r="AE26" s="24">
         <v>854</v>
       </c>
       <c r="AF26" s="19">
-        <v>5243.8874397383925</v>
+        <v>5253</v>
       </c>
     </row>
     <row r="27" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2829,83 +2847,83 @@
         <v>42278</v>
       </c>
       <c r="B27" s="25">
-        <v>117.82178217821782</v>
+        <v>120</v>
       </c>
       <c r="C27" s="24">
         <v>84</v>
       </c>
       <c r="D27" s="19">
-        <v>813.4851485148514</v>
+        <v>851</v>
       </c>
       <c r="E27" s="25"/>
       <c r="F27" s="25">
-        <v>192.2315644383184</v>
+        <v>192</v>
       </c>
       <c r="G27" s="24">
         <v>160</v>
       </c>
       <c r="H27" s="19">
-        <v>1546.1137146795313</v>
+        <v>1510</v>
       </c>
       <c r="I27" s="19"/>
       <c r="J27" s="25">
-        <v>28.571428571428569</v>
+        <v>30</v>
       </c>
       <c r="K27" s="24">
         <v>31</v>
       </c>
       <c r="L27" s="19">
-        <v>157.33333333333326</v>
+        <v>159</v>
       </c>
       <c r="M27" s="19"/>
       <c r="N27" s="25">
-        <v>75.092879256965958</v>
+        <v>80</v>
       </c>
       <c r="O27" s="24">
         <v>84</v>
       </c>
       <c r="P27" s="19">
-        <v>736.13931888544914</v>
+        <v>702</v>
       </c>
       <c r="Q27" s="19"/>
       <c r="R27" s="25">
-        <v>123.70481927710843</v>
+        <v>124</v>
       </c>
       <c r="S27" s="24">
         <v>140</v>
       </c>
       <c r="T27" s="19">
-        <v>758.63253012048176</v>
+        <v>764</v>
       </c>
       <c r="U27" s="19"/>
       <c r="V27" s="25">
-        <v>306.95738724727835</v>
+        <v>312</v>
       </c>
       <c r="W27" s="24">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="X27" s="19">
-        <v>1153.6594090202175</v>
+        <v>1178</v>
       </c>
       <c r="Y27" s="19"/>
       <c r="Z27" s="25">
-        <v>29.826923076923077</v>
+        <v>29</v>
       </c>
       <c r="AA27" s="24">
         <v>36</v>
       </c>
       <c r="AB27" s="19">
-        <v>167.73076923076914</v>
+        <v>189</v>
       </c>
       <c r="AC27" s="19"/>
       <c r="AD27" s="25">
-        <v>874.20678404624061</v>
+        <v>887</v>
       </c>
       <c r="AE27" s="24">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="AF27" s="19">
-        <v>5333.094223784633</v>
+        <v>5353</v>
       </c>
     </row>
     <row r="28" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2913,83 +2931,83 @@
         <v>42309</v>
       </c>
       <c r="B28" s="25">
-        <v>98.019801980198025</v>
+        <v>101</v>
       </c>
       <c r="C28" s="24">
         <v>89</v>
       </c>
       <c r="D28" s="19">
-        <v>822.50495049504946</v>
+        <v>863</v>
       </c>
       <c r="E28" s="25"/>
       <c r="F28" s="25">
-        <v>166.42866988283942</v>
+        <v>166</v>
       </c>
       <c r="G28" s="24">
         <v>153</v>
       </c>
       <c r="H28" s="19">
-        <v>1559.5423845623707</v>
+        <v>1523</v>
       </c>
       <c r="I28" s="19"/>
       <c r="J28" s="25">
-        <v>22.857142857142858</v>
+        <v>24</v>
       </c>
       <c r="K28" s="24">
         <v>24</v>
       </c>
       <c r="L28" s="19">
-        <v>156.19047619047612</v>
+        <v>159</v>
       </c>
       <c r="M28" s="19"/>
       <c r="N28" s="25">
-        <v>84.845201238390104</v>
+        <v>91</v>
       </c>
       <c r="O28" s="24">
         <v>75</v>
       </c>
       <c r="P28" s="19">
-        <v>745.98452012383927</v>
+        <v>718</v>
       </c>
       <c r="Q28" s="19"/>
       <c r="R28" s="25">
-        <v>122.59036144578313</v>
+        <v>123</v>
       </c>
       <c r="S28" s="24">
         <v>97</v>
       </c>
       <c r="T28" s="19">
-        <v>784.22289156626493</v>
+        <v>790</v>
       </c>
       <c r="U28" s="19"/>
       <c r="V28" s="25">
-        <v>275.87309486780714</v>
+        <v>281</v>
       </c>
       <c r="W28" s="24">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="X28" s="19">
-        <v>1208.5325038880246</v>
+        <v>1236</v>
       </c>
       <c r="Y28" s="19"/>
       <c r="Z28" s="25">
-        <v>18.98076923076923</v>
+        <v>18</v>
       </c>
       <c r="AA28" s="24">
         <v>20</v>
       </c>
       <c r="AB28" s="19">
-        <v>166.71153846153837</v>
+        <v>187</v>
       </c>
       <c r="AC28" s="19"/>
       <c r="AD28" s="25">
-        <v>789.59504150292992</v>
+        <v>804</v>
       </c>
       <c r="AE28" s="24">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="AF28" s="19">
-        <v>5443.6892652875631</v>
+        <v>5476</v>
       </c>
     </row>
     <row r="29" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2997,83 +3015,83 @@
         <v>42339</v>
       </c>
       <c r="B29" s="25">
-        <v>98.019801980198025</v>
+        <v>101</v>
       </c>
       <c r="C29" s="24">
         <v>78</v>
       </c>
       <c r="D29" s="19">
-        <v>842.52475247524751</v>
+        <v>886</v>
       </c>
       <c r="E29" s="25"/>
       <c r="F29" s="25">
-        <v>158.68780151619572</v>
+        <v>159</v>
       </c>
       <c r="G29" s="24">
         <v>154</v>
       </c>
       <c r="H29" s="19">
-        <v>1564.2301860785665</v>
+        <v>1528</v>
       </c>
       <c r="I29" s="19"/>
       <c r="J29" s="25">
-        <v>25.714285714285712</v>
+        <v>27</v>
       </c>
       <c r="K29" s="24">
         <v>27</v>
       </c>
       <c r="L29" s="19">
-        <v>154.90476190476184</v>
+        <v>159</v>
       </c>
       <c r="M29" s="19"/>
       <c r="N29" s="25">
-        <v>70.216718266253878</v>
+        <v>75</v>
       </c>
       <c r="O29" s="24">
         <v>78</v>
       </c>
       <c r="P29" s="19">
-        <v>738.20123839009318</v>
+        <v>715</v>
       </c>
       <c r="Q29" s="19"/>
       <c r="R29" s="25">
-        <v>96.9578313253012</v>
+        <v>97</v>
       </c>
       <c r="S29" s="24">
         <v>83</v>
       </c>
       <c r="T29" s="19">
-        <v>798.18072289156612</v>
+        <v>804</v>
       </c>
       <c r="U29" s="19"/>
       <c r="V29" s="25">
-        <v>263.24510108864695</v>
+        <v>267</v>
       </c>
       <c r="W29" s="24">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="X29" s="19">
-        <v>1240.7776049766717</v>
+        <v>1270</v>
       </c>
       <c r="Y29" s="19"/>
       <c r="Z29" s="25">
-        <v>18.076923076923077</v>
+        <v>17</v>
       </c>
       <c r="AA29" s="24">
         <v>27</v>
       </c>
       <c r="AB29" s="19">
-        <v>157.78846153846143</v>
+        <v>177</v>
       </c>
       <c r="AC29" s="19"/>
       <c r="AD29" s="25">
-        <v>730.91846296780466</v>
+        <v>743</v>
       </c>
       <c r="AE29" s="24">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="AF29" s="19">
-        <v>5496.6077282553679</v>
+        <v>5539</v>
       </c>
     </row>
     <row r="30" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3081,83 +3099,83 @@
         <v>42370</v>
       </c>
       <c r="B30" s="25">
-        <v>68.316831683168317</v>
+        <v>70</v>
       </c>
       <c r="C30" s="24">
         <v>80</v>
       </c>
       <c r="D30" s="19">
-        <v>830.8415841584158</v>
+        <v>876</v>
       </c>
       <c r="E30" s="25"/>
       <c r="F30" s="25">
-        <v>159.97794624396968</v>
+        <v>160</v>
       </c>
       <c r="G30" s="24">
         <v>143</v>
       </c>
       <c r="H30" s="19">
-        <v>1581.2081323225361</v>
+        <v>1545</v>
       </c>
       <c r="I30" s="20"/>
       <c r="J30" s="25">
-        <v>28.571428571428569</v>
+        <v>30</v>
       </c>
       <c r="K30" s="24">
         <v>15</v>
       </c>
       <c r="L30" s="19">
-        <v>168.47619047619042</v>
+        <v>174</v>
       </c>
       <c r="M30" s="20"/>
       <c r="N30" s="25">
-        <v>69.241486068111456</v>
+        <v>74</v>
       </c>
       <c r="O30" s="24">
         <v>61</v>
       </c>
       <c r="P30" s="19">
-        <v>746.44272445820468</v>
+        <v>728</v>
       </c>
       <c r="Q30" s="20"/>
       <c r="R30" s="25">
-        <v>85.813253012048193</v>
+        <v>86</v>
       </c>
       <c r="S30" s="24">
         <v>82</v>
       </c>
       <c r="T30" s="19">
-        <v>801.99397590361434</v>
+        <v>808</v>
       </c>
       <c r="U30" s="20"/>
       <c r="V30" s="25">
-        <v>241.87465007776049</v>
+        <v>246</v>
       </c>
       <c r="W30" s="24">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="X30" s="19">
-        <v>1264.6522550544321</v>
+        <v>1293</v>
       </c>
       <c r="Y30" s="20"/>
       <c r="Z30" s="25">
-        <v>13.557692307692307</v>
+        <v>13</v>
       </c>
       <c r="AA30" s="24">
         <v>18</v>
       </c>
       <c r="AB30" s="19">
-        <v>153.34615384615375</v>
+        <v>172</v>
       </c>
       <c r="AC30" s="20"/>
       <c r="AD30" s="25">
-        <v>667.353287964179</v>
+        <v>679</v>
       </c>
       <c r="AE30" s="24">
-        <v>617</v>
+        <v>622</v>
       </c>
       <c r="AF30" s="19">
-        <v>5546.9610162195468</v>
+        <v>5596</v>
       </c>
     </row>
     <row r="31" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3165,83 +3183,83 @@
         <v>42401</v>
       </c>
       <c r="B31" s="25">
-        <v>58.415841584158414</v>
+        <v>60</v>
       </c>
       <c r="C31" s="24">
         <v>41</v>
       </c>
       <c r="D31" s="19">
-        <v>848.25742574257424</v>
+        <v>895</v>
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="25">
-        <v>114.82288077188146</v>
+        <v>115</v>
       </c>
       <c r="G31" s="24">
         <v>128</v>
       </c>
       <c r="H31" s="19">
-        <v>1568.0310130944176</v>
+        <v>1532</v>
       </c>
       <c r="I31" s="20"/>
       <c r="J31" s="25">
-        <v>12.38095238095238</v>
+        <v>13</v>
       </c>
       <c r="K31" s="24">
         <v>18</v>
       </c>
       <c r="L31" s="19">
-        <v>162.8571428571428</v>
+        <v>169</v>
       </c>
       <c r="M31" s="20"/>
       <c r="N31" s="25">
-        <v>55.588235294117652</v>
+        <v>59</v>
       </c>
       <c r="O31" s="24">
         <v>75</v>
       </c>
       <c r="P31" s="19">
-        <v>727.03095975232236</v>
+        <v>712</v>
       </c>
       <c r="Q31" s="20"/>
       <c r="R31" s="25">
-        <v>78.012048192771076</v>
+        <v>78</v>
       </c>
       <c r="S31" s="24">
         <v>81</v>
       </c>
       <c r="T31" s="19">
-        <v>799.00602409638543</v>
+        <v>805</v>
       </c>
       <c r="U31" s="20"/>
       <c r="V31" s="25">
-        <v>191.36267496111975</v>
+        <v>195</v>
       </c>
       <c r="W31" s="24">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="X31" s="19">
-        <v>1244.0149300155517</v>
+        <v>1272</v>
       </c>
       <c r="Y31" s="20"/>
       <c r="Z31" s="25">
-        <v>17.173076923076923</v>
+        <v>16</v>
       </c>
       <c r="AA31" s="24">
         <v>9</v>
       </c>
       <c r="AB31" s="19">
-        <v>161.51923076923069</v>
+        <v>179</v>
       </c>
       <c r="AC31" s="20"/>
       <c r="AD31" s="25">
-        <v>527.75571010807766</v>
+        <v>536</v>
       </c>
       <c r="AE31" s="24">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="AF31" s="19">
-        <v>5510.7167263276242</v>
+        <v>5564</v>
       </c>
     </row>
     <row r="32" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3249,83 +3267,83 @@
         <v>42430</v>
       </c>
       <c r="B32" s="25">
-        <v>63.366336633663366</v>
+        <v>65</v>
       </c>
       <c r="C32" s="24">
         <v>45</v>
       </c>
       <c r="D32" s="19">
-        <v>866.62376237623766</v>
+        <v>915</v>
       </c>
       <c r="E32" s="25"/>
       <c r="F32" s="25">
-        <v>89.019986216402472</v>
+        <v>89</v>
       </c>
       <c r="G32" s="24">
         <v>112</v>
       </c>
       <c r="H32" s="19">
-        <v>1545.0509993108201</v>
+        <v>1509</v>
       </c>
       <c r="I32" s="20"/>
       <c r="J32" s="25">
-        <v>10.476190476190476</v>
+        <v>11</v>
       </c>
       <c r="K32" s="24">
         <v>14</v>
       </c>
       <c r="L32" s="19">
-        <v>159.33333333333329</v>
+        <v>166</v>
       </c>
       <c r="M32" s="20"/>
       <c r="N32" s="25">
-        <v>52.662538699690408</v>
+        <v>56</v>
       </c>
       <c r="O32" s="24">
         <v>65</v>
       </c>
       <c r="P32" s="19">
-        <v>714.69349845201282</v>
+        <v>703</v>
       </c>
       <c r="Q32" s="20"/>
       <c r="R32" s="25">
-        <v>60.180722891566262</v>
+        <v>60</v>
       </c>
       <c r="S32" s="24">
         <v>58</v>
       </c>
       <c r="T32" s="19">
-        <v>801.18674698795166</v>
+        <v>807</v>
       </c>
       <c r="U32" s="20"/>
       <c r="V32" s="25">
-        <v>207.87620528771384</v>
+        <v>211</v>
       </c>
       <c r="W32" s="24">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="X32" s="19">
-        <v>1261.8911353032656</v>
+        <v>1282</v>
       </c>
       <c r="Y32" s="20"/>
       <c r="Z32" s="25">
-        <v>16.26923076923077</v>
+        <v>16</v>
       </c>
       <c r="AA32" s="24">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB32" s="19">
-        <v>167.78846153846146</v>
+        <v>186</v>
       </c>
       <c r="AC32" s="20"/>
       <c r="AD32" s="25">
-        <v>499.85121097445756</v>
+        <v>508</v>
       </c>
       <c r="AE32" s="24">
-        <v>494</v>
+        <v>504</v>
       </c>
       <c r="AF32" s="19">
-        <v>5516.5679373020821</v>
+        <v>5568</v>
       </c>
     </row>
     <row r="33" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3333,83 +3351,83 @@
         <v>42461</v>
       </c>
       <c r="B33" s="25">
-        <v>41.584158415841586</v>
-      </c>
-      <c r="C33" s="25">
+        <v>43</v>
+      </c>
+      <c r="C33" s="24">
         <v>38</v>
       </c>
       <c r="D33" s="19">
-        <v>870.20792079207922</v>
+        <v>920</v>
       </c>
       <c r="E33" s="25"/>
       <c r="F33" s="25">
-        <v>69.667815299793247</v>
-      </c>
-      <c r="G33" s="25">
+        <v>70</v>
+      </c>
+      <c r="G33" s="24">
         <v>118</v>
       </c>
       <c r="H33" s="19">
-        <v>1496.7188146106134</v>
+        <v>1461</v>
       </c>
       <c r="I33" s="20"/>
       <c r="J33" s="25">
-        <v>15.238095238095237</v>
-      </c>
-      <c r="K33" s="25">
+        <v>16</v>
+      </c>
+      <c r="K33" s="24">
         <v>25</v>
       </c>
       <c r="L33" s="19">
-        <v>149.57142857142853</v>
+        <v>157</v>
       </c>
       <c r="M33" s="20"/>
       <c r="N33" s="25">
-        <v>43.88544891640867</v>
-      </c>
-      <c r="O33" s="25">
+        <v>47</v>
+      </c>
+      <c r="O33" s="24">
         <v>53</v>
       </c>
       <c r="P33" s="19">
-        <v>705.5789473684215</v>
+        <v>697</v>
       </c>
       <c r="Q33" s="20"/>
       <c r="R33" s="25">
-        <v>42.349397590361441</v>
-      </c>
-      <c r="S33" s="25">
+        <v>42</v>
+      </c>
+      <c r="S33" s="24">
         <v>75</v>
       </c>
       <c r="T33" s="19">
-        <v>768.53614457831316</v>
+        <v>774</v>
       </c>
       <c r="U33" s="20"/>
       <c r="V33" s="25">
-        <v>176.79191290824261</v>
-      </c>
-      <c r="W33" s="25">
-        <v>197</v>
+        <v>180</v>
+      </c>
+      <c r="W33" s="24">
+        <v>204</v>
       </c>
       <c r="X33" s="19">
-        <v>1241.6830482115083</v>
+        <v>1258</v>
       </c>
       <c r="Y33" s="20"/>
       <c r="Z33" s="25">
-        <v>9.0384615384615383</v>
-      </c>
-      <c r="AA33" s="25">
+        <v>9</v>
+      </c>
+      <c r="AA33" s="24">
         <v>16</v>
       </c>
       <c r="AB33" s="19">
-        <v>160.82692307692301</v>
+        <v>179</v>
       </c>
       <c r="AC33" s="20"/>
       <c r="AD33" s="25">
-        <v>398.55528990720427</v>
-      </c>
-      <c r="AE33" s="25">
-        <v>522</v>
+        <v>407</v>
+      </c>
+      <c r="AE33" s="24">
+        <v>529</v>
       </c>
       <c r="AF33" s="19">
-        <v>5393.1232272092866</v>
+        <v>5446</v>
       </c>
     </row>
     <row r="34" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3417,83 +3435,83 @@
         <v>42491</v>
       </c>
       <c r="B34" s="25">
-        <v>44.554455445544555</v>
+        <v>46</v>
       </c>
       <c r="C34" s="25">
         <v>59</v>
       </c>
       <c r="D34" s="19">
-        <v>855.76237623762381</v>
+        <v>907</v>
       </c>
       <c r="E34" s="25"/>
       <c r="F34" s="25">
-        <v>65.797381116471399</v>
+        <v>66</v>
       </c>
       <c r="G34" s="25">
         <v>139</v>
       </c>
       <c r="H34" s="19">
-        <v>1423.5161957270848</v>
+        <v>1388</v>
       </c>
       <c r="I34" s="20"/>
       <c r="J34" s="25">
-        <v>14.285714285714285</v>
+        <v>15</v>
       </c>
       <c r="K34" s="25">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L34" s="19">
-        <v>154.8571428571428</v>
+        <v>162</v>
       </c>
       <c r="M34" s="20"/>
       <c r="N34" s="25">
-        <v>44.860681114551085</v>
+        <v>48</v>
       </c>
       <c r="O34" s="25">
         <v>51</v>
       </c>
       <c r="P34" s="19">
-        <v>699.43962848297258</v>
+        <v>694</v>
       </c>
       <c r="Q34" s="20"/>
       <c r="R34" s="25">
-        <v>60.180722891566262</v>
+        <v>60</v>
       </c>
       <c r="S34" s="25">
         <v>92</v>
       </c>
       <c r="T34" s="19">
-        <v>736.71686746987939</v>
+        <v>742</v>
       </c>
       <c r="U34" s="20"/>
       <c r="V34" s="25">
-        <v>162.22115085536547</v>
+        <v>165</v>
       </c>
       <c r="W34" s="25">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="X34" s="19">
-        <v>1235.9041990668738</v>
+        <v>1248</v>
       </c>
       <c r="Y34" s="20"/>
       <c r="Z34" s="25">
-        <v>9.0384615384615383</v>
+        <v>9</v>
       </c>
       <c r="AA34" s="25">
         <v>26</v>
       </c>
       <c r="AB34" s="19">
-        <v>143.86538461538456</v>
+        <v>162</v>
       </c>
       <c r="AC34" s="20"/>
       <c r="AD34" s="25">
-        <v>400.9385672476746</v>
+        <v>409</v>
       </c>
       <c r="AE34" s="25">
-        <v>544</v>
+        <v>552</v>
       </c>
       <c r="AF34" s="19">
-        <v>5250.0617944569613</v>
+        <v>5303</v>
       </c>
     </row>
     <row r="35" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3501,83 +3519,83 @@
         <v>42522</v>
       </c>
       <c r="B35" s="25">
-        <v>39.603960396039604</v>
+        <v>41</v>
       </c>
       <c r="C35" s="25">
         <v>54</v>
       </c>
       <c r="D35" s="19">
-        <v>841.36633663366342</v>
+        <v>894</v>
       </c>
       <c r="E35" s="25"/>
       <c r="F35" s="25">
-        <v>64.50723638869745</v>
+        <v>65</v>
       </c>
       <c r="G35" s="25">
         <v>99</v>
       </c>
       <c r="H35" s="19">
-        <v>1389.0234321157823</v>
+        <v>1354</v>
       </c>
       <c r="I35" s="20"/>
       <c r="J35" s="25">
-        <v>17.142857142857142</v>
+        <v>18</v>
       </c>
       <c r="K35" s="25">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L35" s="19">
-        <v>145.99999999999994</v>
+        <v>153</v>
       </c>
       <c r="M35" s="20"/>
       <c r="N35" s="25">
-        <v>38.034055727554183</v>
+        <v>40</v>
       </c>
       <c r="O35" s="25">
         <v>41</v>
       </c>
       <c r="P35" s="19">
-        <v>696.47368421052681</v>
+        <v>693</v>
       </c>
       <c r="Q35" s="20"/>
       <c r="R35" s="25">
-        <v>56.837349397590359</v>
+        <v>57</v>
       </c>
       <c r="S35" s="25">
         <v>81</v>
       </c>
       <c r="T35" s="19">
-        <v>712.55421686746979</v>
+        <v>718</v>
       </c>
       <c r="U35" s="20"/>
       <c r="V35" s="25">
-        <v>195.24821150855365</v>
+        <v>198</v>
       </c>
       <c r="W35" s="25">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="X35" s="19">
-        <v>1235.1524105754274</v>
+        <v>1238</v>
       </c>
       <c r="Y35" s="20"/>
       <c r="Z35" s="25">
-        <v>9.9423076923076916</v>
+        <v>10</v>
       </c>
       <c r="AA35" s="25">
         <v>24</v>
       </c>
       <c r="AB35" s="19">
-        <v>129.80769230769224</v>
+        <v>148</v>
       </c>
       <c r="AC35" s="20"/>
       <c r="AD35" s="25">
-        <v>421.31597825360006</v>
+        <v>429</v>
       </c>
       <c r="AE35" s="25">
-        <v>521</v>
+        <v>534</v>
       </c>
       <c r="AF35" s="19">
-        <v>5150.3777727105617</v>
+        <v>5198</v>
       </c>
     </row>
     <row r="36" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3585,83 +3603,83 @@
         <v>42552</v>
       </c>
       <c r="B36" s="25">
-        <v>43.564356435643568</v>
+        <v>45</v>
       </c>
       <c r="C36" s="25">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D36" s="19">
-        <v>830.93069306930704</v>
+        <v>883</v>
       </c>
       <c r="E36" s="25"/>
       <c r="F36" s="25">
-        <v>65.797381116471399</v>
+        <v>66</v>
       </c>
       <c r="G36" s="25">
         <v>100</v>
       </c>
       <c r="H36" s="19">
-        <v>1354.8208132322536</v>
+        <v>1320</v>
       </c>
       <c r="I36" s="20"/>
       <c r="J36" s="25">
-        <v>25.714285714285712</v>
+        <v>27</v>
       </c>
       <c r="K36" s="25">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="L36" s="19">
-        <v>156.71428571428567</v>
+        <v>161</v>
       </c>
       <c r="M36" s="20"/>
       <c r="N36" s="25">
-        <v>30.232198142414862</v>
+        <v>32</v>
       </c>
       <c r="O36" s="25">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P36" s="19">
-        <v>671.70588235294167</v>
+        <v>669</v>
       </c>
       <c r="Q36" s="20"/>
       <c r="R36" s="25">
-        <v>64.638554216867462</v>
+        <v>65</v>
       </c>
       <c r="S36" s="25">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="T36" s="19">
-        <v>689.19277108433721</v>
+        <v>693</v>
       </c>
       <c r="U36" s="20"/>
       <c r="V36" s="25">
-        <v>194.27682737169516</v>
+        <v>197</v>
       </c>
       <c r="W36" s="25">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="X36" s="19">
-        <v>1270.4292379471226</v>
+        <v>1260</v>
       </c>
       <c r="Y36" s="20"/>
       <c r="Z36" s="25">
-        <v>10.846153846153845</v>
+        <v>10</v>
       </c>
       <c r="AA36" s="25">
         <v>23</v>
       </c>
       <c r="AB36" s="19">
-        <v>117.65384615384608</v>
+        <v>135</v>
       </c>
       <c r="AC36" s="20"/>
       <c r="AD36" s="25">
-        <v>435.06975684353199</v>
+        <v>442</v>
       </c>
       <c r="AE36" s="25">
-        <v>494</v>
+        <v>519</v>
       </c>
       <c r="AF36" s="19">
-        <v>5091.4475295540933</v>
+        <v>5121</v>
       </c>
     </row>
     <row r="37" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3669,83 +3687,83 @@
         <v>42583</v>
       </c>
       <c r="B37" s="25">
-        <v>58.415841584158414</v>
+        <v>56</v>
       </c>
       <c r="C37" s="25">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D37" s="19">
-        <v>813.34653465346548</v>
+        <v>858</v>
       </c>
       <c r="E37" s="25"/>
       <c r="F37" s="25">
-        <v>101.92143349414197</v>
+        <v>102</v>
       </c>
       <c r="G37" s="25">
         <v>116</v>
       </c>
       <c r="H37" s="19">
-        <v>1340.7422467263955</v>
+        <v>1306</v>
       </c>
       <c r="I37" s="20"/>
       <c r="J37" s="25">
-        <v>15.238095238095237</v>
+        <v>16</v>
       </c>
       <c r="K37" s="25">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L37" s="19">
-        <v>148.95238095238091</v>
+        <v>152</v>
       </c>
       <c r="M37" s="20"/>
       <c r="N37" s="25">
-        <v>34.133126934984524</v>
+        <v>36</v>
       </c>
       <c r="O37" s="25">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="P37" s="19">
-        <v>651.83900928792616</v>
+        <v>649</v>
       </c>
       <c r="Q37" s="20"/>
       <c r="R37" s="25">
-        <v>78.012048192771076</v>
+        <v>78</v>
       </c>
       <c r="S37" s="25">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="T37" s="19">
-        <v>670.2048192771083</v>
+        <v>665</v>
       </c>
       <c r="U37" s="20"/>
       <c r="V37" s="25">
-        <v>239.93188180404354</v>
+        <v>243</v>
       </c>
       <c r="W37" s="25">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="X37" s="19">
-        <v>1313.3611197511661</v>
+        <v>1280</v>
       </c>
       <c r="Y37" s="20"/>
       <c r="Z37" s="25">
-        <v>12.653846153846153</v>
+        <v>12</v>
       </c>
       <c r="AA37" s="25">
         <v>12</v>
       </c>
       <c r="AB37" s="19">
-        <v>118.30769230769224</v>
+        <v>135</v>
       </c>
       <c r="AC37" s="20"/>
       <c r="AD37" s="25">
-        <v>540.30627340204092</v>
+        <v>543</v>
       </c>
       <c r="AE37" s="25">
-        <v>575</v>
+        <v>619</v>
       </c>
       <c r="AF37" s="19">
-        <v>5056.7538029561347</v>
+        <v>5045</v>
       </c>
     </row>
     <row r="38" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3753,83 +3771,83 @@
         <v>42614</v>
       </c>
       <c r="B38" s="25">
-        <v>51.485148514851488</v>
+        <v>48</v>
       </c>
       <c r="C38" s="25">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D38" s="19">
-        <v>808.831683168317</v>
+        <v>840</v>
       </c>
       <c r="E38" s="25"/>
       <c r="F38" s="25">
-        <v>91.600275671950371</v>
+        <v>92</v>
       </c>
       <c r="G38" s="25">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H38" s="19">
-        <v>1324.3425223983459</v>
+        <v>1287</v>
       </c>
       <c r="I38" s="20"/>
       <c r="J38" s="25">
-        <v>18.095238095238095</v>
+        <v>20</v>
       </c>
       <c r="K38" s="25">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L38" s="19">
-        <v>151.04761904761901</v>
+        <v>158</v>
       </c>
       <c r="M38" s="20"/>
       <c r="N38" s="25">
-        <v>36.083591331269353</v>
+        <v>39</v>
       </c>
       <c r="O38" s="25">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P38" s="19">
-        <v>642.92260061919546</v>
+        <v>642</v>
       </c>
       <c r="Q38" s="20"/>
       <c r="R38" s="25">
-        <v>64.638554216867462</v>
+        <v>66</v>
       </c>
       <c r="S38" s="25">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="T38" s="19">
-        <v>659.84337349397572</v>
+        <v>649</v>
       </c>
       <c r="U38" s="20"/>
       <c r="V38" s="25">
-        <v>250.61710730948678</v>
+        <v>254</v>
       </c>
       <c r="W38" s="25">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="X38" s="19">
-        <v>1378.9782270606529</v>
+        <v>1334</v>
       </c>
       <c r="Y38" s="20"/>
       <c r="Z38" s="25">
-        <v>11.75</v>
+        <v>9</v>
       </c>
       <c r="AA38" s="25">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB38" s="19">
-        <v>116.05769230769224</v>
+        <v>129</v>
       </c>
       <c r="AC38" s="20"/>
       <c r="AD38" s="25">
-        <v>524.26991513966357</v>
+        <v>528</v>
       </c>
       <c r="AE38" s="25">
-        <v>499</v>
+        <v>534</v>
       </c>
       <c r="AF38" s="19">
-        <v>5082.0237180957984</v>
+        <v>5039</v>
       </c>
     </row>
     <row r="39" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3837,237 +3855,405 @@
         <v>42644</v>
       </c>
       <c r="B39" s="25">
-        <v>65.346534653465341</v>
+        <v>60</v>
       </c>
       <c r="C39" s="25">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D39" s="19">
-        <v>813.17821782178237</v>
+        <v>820</v>
       </c>
       <c r="E39" s="25"/>
       <c r="F39" s="25">
-        <v>86.439696760854574</v>
+        <v>86</v>
       </c>
       <c r="G39" s="25">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="H39" s="19">
-        <v>1296.7822191592004</v>
-      </c>
-      <c r="I39" s="20"/>
+        <v>1245</v>
+      </c>
+      <c r="I39" s="19"/>
       <c r="J39" s="25">
-        <v>21.904761904761905</v>
+        <v>18</v>
       </c>
       <c r="K39" s="25">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L39" s="19">
-        <v>152.95238095238091</v>
-      </c>
-      <c r="M39" s="20"/>
+        <v>151</v>
+      </c>
+      <c r="M39" s="19"/>
       <c r="N39" s="25">
-        <v>39.984520123839012</v>
+        <v>40</v>
       </c>
       <c r="O39" s="25">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="P39" s="19">
-        <v>635.90712074303451</v>
-      </c>
-      <c r="Q39" s="20"/>
+        <v>627</v>
+      </c>
+      <c r="Q39" s="19"/>
       <c r="R39" s="25">
-        <v>76.897590361445779</v>
+        <v>77</v>
       </c>
       <c r="S39" s="25">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T39" s="19">
-        <v>671.74096385542146</v>
-      </c>
-      <c r="U39" s="20"/>
+        <v>662</v>
+      </c>
+      <c r="U39" s="19"/>
       <c r="V39" s="25">
-        <v>281.70139968895802</v>
+        <v>281</v>
       </c>
       <c r="W39" s="25">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="X39" s="19">
-        <v>1468.6796267496109</v>
-      </c>
-      <c r="Y39" s="20"/>
+        <v>1425</v>
+      </c>
+      <c r="Y39" s="19"/>
       <c r="Z39" s="25">
-        <v>13.557692307692307</v>
+        <v>12</v>
       </c>
       <c r="AA39" s="25">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="AB39" s="19">
-        <v>114.61538461538453</v>
-      </c>
-      <c r="AC39" s="20"/>
+        <v>112</v>
+      </c>
+      <c r="AC39" s="19"/>
       <c r="AD39" s="25">
-        <v>585.83219580101695</v>
+        <v>574</v>
       </c>
       <c r="AE39" s="25">
-        <v>514</v>
+        <v>571</v>
       </c>
       <c r="AF39" s="19">
-        <v>5153.8559138968158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:32" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5042</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>42675</v>
       </c>
       <c r="B40" s="25">
-        <v>68.316831683168317</v>
+        <v>69</v>
       </c>
       <c r="C40" s="25">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D40" s="19">
-        <v>814.49504950495066</v>
+        <v>809</v>
       </c>
       <c r="E40" s="25"/>
       <c r="F40" s="25">
-        <v>89.019986216402472</v>
+        <v>89</v>
       </c>
       <c r="G40" s="25">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H40" s="19">
-        <v>1277.8022053756029</v>
-      </c>
-      <c r="I40" s="20"/>
+        <v>1228</v>
+      </c>
+      <c r="I40" s="19"/>
       <c r="J40" s="25">
-        <v>25.714285714285712</v>
+        <v>27</v>
       </c>
       <c r="K40" s="25">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L40" s="19">
-        <v>151.66666666666663</v>
-      </c>
-      <c r="M40" s="20"/>
+        <v>154</v>
+      </c>
+      <c r="M40" s="19"/>
       <c r="N40" s="25">
-        <v>44.860681114551085</v>
+        <v>47</v>
       </c>
       <c r="O40" s="25">
         <v>58</v>
       </c>
       <c r="P40" s="19">
-        <v>622.7678018575856</v>
-      </c>
-      <c r="Q40" s="20"/>
+        <v>616</v>
+      </c>
+      <c r="Q40" s="19"/>
       <c r="R40" s="25">
-        <v>81.355421686746979</v>
+        <v>74</v>
       </c>
       <c r="S40" s="25">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="T40" s="19">
-        <v>675.09638554216849</v>
-      </c>
-      <c r="U40" s="20"/>
+        <v>662</v>
+      </c>
+      <c r="U40" s="19"/>
       <c r="V40" s="25">
-        <v>310.84292379471231</v>
+        <v>321</v>
       </c>
       <c r="W40" s="25">
         <v>212</v>
       </c>
       <c r="X40" s="19">
-        <v>1567.5225505443232</v>
-      </c>
-      <c r="Y40" s="20"/>
+        <v>1534</v>
+      </c>
+      <c r="Y40" s="19"/>
       <c r="Z40" s="25">
-        <v>14.461538461538462</v>
+        <v>16</v>
       </c>
       <c r="AA40" s="25">
+        <v>21</v>
+      </c>
+      <c r="AB40" s="19">
+        <v>107</v>
+      </c>
+      <c r="AC40" s="19"/>
+      <c r="AD40" s="25">
+        <v>643</v>
+      </c>
+      <c r="AE40" s="25">
+        <v>575</v>
+      </c>
+      <c r="AF40" s="19">
+        <v>5110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>42705</v>
+      </c>
+      <c r="B41" s="25">
+        <v>66</v>
+      </c>
+      <c r="C41" s="25">
+        <v>67</v>
+      </c>
+      <c r="D41" s="19">
+        <v>808</v>
+      </c>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25">
+        <v>123</v>
+      </c>
+      <c r="G41" s="25">
+        <v>107</v>
+      </c>
+      <c r="H41" s="19">
+        <v>1244</v>
+      </c>
+      <c r="I41" s="19"/>
+      <c r="J41" s="25">
+        <v>29</v>
+      </c>
+      <c r="K41" s="25">
+        <v>27</v>
+      </c>
+      <c r="L41" s="19">
+        <v>156</v>
+      </c>
+      <c r="M41" s="19"/>
+      <c r="N41" s="25">
+        <v>49</v>
+      </c>
+      <c r="O41" s="25">
+        <v>55</v>
+      </c>
+      <c r="P41" s="19">
+        <v>610</v>
+      </c>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="25">
+        <v>98</v>
+      </c>
+      <c r="S41" s="25">
+        <v>65</v>
+      </c>
+      <c r="T41" s="19">
+        <v>695</v>
+      </c>
+      <c r="U41" s="19"/>
+      <c r="V41" s="25">
+        <v>347</v>
+      </c>
+      <c r="W41" s="25">
+        <v>208</v>
+      </c>
+      <c r="X41" s="19">
+        <v>1673</v>
+      </c>
+      <c r="Y41" s="19"/>
+      <c r="Z41" s="25">
+        <v>16</v>
+      </c>
+      <c r="AA41" s="25">
         <v>20</v>
       </c>
-      <c r="AB40" s="19">
-        <v>109.07692307692298</v>
-      </c>
-      <c r="AC40" s="20"/>
-      <c r="AD40" s="25">
-        <v>634.57166867140529</v>
-      </c>
-      <c r="AE40" s="25">
-        <v>570</v>
-      </c>
-      <c r="AF40" s="19">
-        <v>5218.4275825682207</v>
-      </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-      <c r="S41" s="10"/>
-      <c r="T41" s="10"/>
-      <c r="U41" s="10"/>
-      <c r="V41" s="10"/>
-      <c r="W41" s="10"/>
-      <c r="X41" s="10"/>
-      <c r="Y41" s="10"/>
-      <c r="Z41" s="10"/>
-      <c r="AA41" s="10"/>
-      <c r="AB41" s="10"/>
-      <c r="AC41" s="10"/>
-      <c r="AD41" s="10"/>
-      <c r="AE41" s="10"/>
-      <c r="AF41" s="10"/>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="7"/>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="7"/>
-      <c r="W42" s="7"/>
-      <c r="X42" s="8"/>
-      <c r="Y42" s="8"/>
-      <c r="Z42" s="7"/>
-      <c r="AA42" s="7"/>
-      <c r="AB42" s="8"/>
-      <c r="AC42" s="8"/>
-      <c r="AD42" s="7"/>
+      <c r="AB41" s="19">
+        <v>103</v>
+      </c>
+      <c r="AC41" s="19"/>
+      <c r="AD41" s="25">
+        <v>728</v>
+      </c>
+      <c r="AE41" s="25">
+        <v>549</v>
+      </c>
+      <c r="AF41" s="19">
+        <v>5289</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B42" s="25">
+        <v>71</v>
+      </c>
+      <c r="C42" s="25">
+        <v>72</v>
+      </c>
+      <c r="D42" s="19">
+        <v>807</v>
+      </c>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25">
+        <v>132</v>
+      </c>
+      <c r="G42" s="25">
+        <v>121</v>
+      </c>
+      <c r="H42" s="19">
+        <v>1255</v>
+      </c>
+      <c r="I42" s="19"/>
+      <c r="J42" s="25">
+        <v>30</v>
+      </c>
+      <c r="K42" s="25">
+        <v>30</v>
+      </c>
+      <c r="L42" s="19">
+        <v>156</v>
+      </c>
+      <c r="M42" s="19"/>
+      <c r="N42" s="25">
+        <v>50</v>
+      </c>
+      <c r="O42" s="25">
+        <v>60</v>
+      </c>
+      <c r="P42" s="19">
+        <v>600</v>
+      </c>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="25">
+        <v>102</v>
+      </c>
+      <c r="S42" s="25">
+        <v>89</v>
+      </c>
+      <c r="T42" s="19">
+        <v>708</v>
+      </c>
+      <c r="U42" s="19"/>
+      <c r="V42" s="25">
+        <v>356</v>
+      </c>
+      <c r="W42" s="25">
+        <v>272</v>
+      </c>
+      <c r="X42" s="19">
+        <v>1757</v>
+      </c>
+      <c r="Y42" s="19"/>
+      <c r="Z42" s="25">
+        <v>19</v>
+      </c>
+      <c r="AA42" s="25">
+        <v>24</v>
+      </c>
+      <c r="AB42" s="19">
+        <v>98</v>
+      </c>
+      <c r="AC42" s="19"/>
+      <c r="AD42" s="25">
+        <v>760</v>
+      </c>
+      <c r="AE42" s="25">
+        <v>668</v>
+      </c>
+      <c r="AF42" s="19">
+        <v>5381</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="10"/>
+      <c r="W43" s="10"/>
+      <c r="X43" s="10"/>
+      <c r="Y43" s="10"/>
+      <c r="Z43" s="10"/>
+      <c r="AA43" s="10"/>
+      <c r="AB43" s="10"/>
+      <c r="AC43" s="10"/>
+      <c r="AD43" s="10"/>
+      <c r="AE43" s="10"/>
+      <c r="AF43" s="10"/>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="7"/>
+      <c r="S44" s="7"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="7"/>
+      <c r="X44" s="8"/>
+      <c r="Y44" s="8"/>
+      <c r="Z44" s="7"/>
+      <c r="AA44" s="7"/>
+      <c r="AB44" s="8"/>
+      <c r="AC44" s="8"/>
+      <c r="AD44" s="7"/>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="T46" s="9"/>
+      <c r="U46" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4090,62 +4276,138 @@
   <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="27">
+        <v>42705</v>
+      </c>
+      <c r="C2" s="27">
+        <v>42736</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="28"/>
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="26">
+        <v>808</v>
+      </c>
+      <c r="C3" s="26">
+        <v>807</v>
+      </c>
+      <c r="D3" s="28">
+        <v>-1</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="28"/>
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="26">
+        <v>1244</v>
+      </c>
+      <c r="C4" s="26">
+        <v>1255</v>
+      </c>
+      <c r="D4" s="28">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="28"/>
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="26">
+        <v>156</v>
+      </c>
+      <c r="C5" s="26">
+        <v>156</v>
+      </c>
+      <c r="D5" s="28">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="28"/>
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="26">
+        <v>610</v>
+      </c>
+      <c r="C6" s="26">
+        <v>600</v>
+      </c>
+      <c r="D6" s="28">
+        <v>-10</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="28"/>
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="26">
+        <v>695</v>
+      </c>
+      <c r="C7" s="26">
+        <v>708</v>
+      </c>
+      <c r="D7" s="28">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="28"/>
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1673</v>
+      </c>
+      <c r="C8" s="26">
+        <v>1757</v>
+      </c>
+      <c r="D8" s="28">
+        <v>84</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="33"/>
+      <c r="A9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="30">
+        <v>103</v>
+      </c>
+      <c r="C9" s="30">
+        <v>98</v>
+      </c>
+      <c r="D9" s="31">
+        <v>-5</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="28"/>
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="26">
+        <v>5289</v>
+      </c>
+      <c r="C10" s="26">
+        <v>5381</v>
+      </c>
+      <c r="D10" s="28">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>